<commit_message>
LBCB 3 Calibration settings.
</commit_message>
<xml_diff>
--- a/Config/Calibrations/Crane Bay ShuntCal LBCB3.xlsx
+++ b/Config/Calibrations/Crane Bay ShuntCal LBCB3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3975" yWindow="3645" windowWidth="26460" windowHeight="15990" tabRatio="677" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="3975" yWindow="3645" windowWidth="26460" windowHeight="15990" tabRatio="677"/>
   </bookViews>
   <sheets>
     <sheet name="LBCB Serial Numbers" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="50">
   <si>
     <t>FACTORY CALIBRATION</t>
   </si>
@@ -187,7 +187,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -503,29 +503,29 @@
     <xf numFmtId="2" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="7" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -535,23 +535,23 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="166" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -565,28 +565,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -826,13 +826,13 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5.8995899999999999</c:v>
+                  <c:v>3.04867</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.22700500000000001</c:v>
+                  <c:v>0.16231799999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-5.3392200000000001</c:v>
+                  <c:v>-2.7215099999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -865,11 +865,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="83598656"/>
-        <c:axId val="43810816"/>
+        <c:axId val="96913088"/>
+        <c:axId val="96913664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83598656"/>
+        <c:axId val="96913088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -943,12 +943,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43810816"/>
+        <c:crossAx val="96913664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43810816"/>
+        <c:axId val="96913664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1032,7 +1032,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83598656"/>
+        <c:crossAx val="96913088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1277,13 +1277,13 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5.9729999999999999</c:v>
+                  <c:v>2.9597000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.16631899999999999</c:v>
+                  <c:v>7.0880299999999993E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-5.6299400000000004</c:v>
+                  <c:v>-2.8110200000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1316,11 +1316,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="43812544"/>
-        <c:axId val="43813120"/>
+        <c:axId val="96915392"/>
+        <c:axId val="96915968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="43812544"/>
+        <c:axId val="96915392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1394,12 +1394,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43813120"/>
+        <c:crossAx val="96915968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43813120"/>
+        <c:axId val="96915968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1483,7 +1483,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43812544"/>
+        <c:crossAx val="96915392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1728,13 +1728,13 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>6.0389999999999997</c:v>
+                  <c:v>2.99234</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.26349699999999998</c:v>
+                  <c:v>0.175562</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-5.5067399999999997</c:v>
+                  <c:v>-2.6374499999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1767,11 +1767,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="43814848"/>
-        <c:axId val="43815424"/>
+        <c:axId val="96917696"/>
+        <c:axId val="96918272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="43814848"/>
+        <c:axId val="96917696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1845,12 +1845,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43815424"/>
+        <c:crossAx val="96918272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43815424"/>
+        <c:axId val="96918272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1934,7 +1934,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43814848"/>
+        <c:crossAx val="96917696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2179,13 +2179,13 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>6.3773400000000002</c:v>
+                  <c:v>3.2391299999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.64461900000000005</c:v>
+                  <c:v>0.440218</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-5.09063</c:v>
+                  <c:v>-2.3597700000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2218,11 +2218,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="43817152"/>
-        <c:axId val="43817728"/>
+        <c:axId val="97894976"/>
+        <c:axId val="97895552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="43817152"/>
+        <c:axId val="97894976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2296,12 +2296,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43817728"/>
+        <c:crossAx val="97895552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43817728"/>
+        <c:axId val="97895552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2385,7 +2385,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43817152"/>
+        <c:crossAx val="97894976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2630,13 +2630,13 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>6.3040200000000004</c:v>
+                  <c:v>3.1473599999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.53485099999999997</c:v>
+                  <c:v>0.282163</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-5.2269399999999999</c:v>
+                  <c:v>-2.5787399999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2669,11 +2669,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="44655168"/>
-        <c:axId val="44655744"/>
+        <c:axId val="97897280"/>
+        <c:axId val="97897856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44655168"/>
+        <c:axId val="97897280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2747,12 +2747,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44655744"/>
+        <c:crossAx val="97897856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44655744"/>
+        <c:axId val="97897856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2836,7 +2836,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44655168"/>
+        <c:crossAx val="97897280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3081,13 +3081,13 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>6.2019099999999998</c:v>
+                  <c:v>3.1657099999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.466248</c:v>
+                  <c:v>0.261407</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-5.2678000000000003</c:v>
+                  <c:v>-2.6425100000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3120,11 +3120,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="44657472"/>
-        <c:axId val="44658048"/>
+        <c:axId val="97899584"/>
+        <c:axId val="97900160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44657472"/>
+        <c:axId val="97899584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3198,12 +3198,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44658048"/>
+        <c:crossAx val="97900160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44658048"/>
+        <c:axId val="97900160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3287,7 +3287,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44657472"/>
+        <c:crossAx val="97899584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3894,71 +3894,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="54.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="57" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="58"/>
-    </row>
-    <row r="3" spans="1:2" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A3" s="59" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="60" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>32.951978266894599</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A4" s="61" t="s">
         <v>32</v>
       </c>
       <c r="B4" s="62" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>33.135271036646103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A5" s="61" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="62" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>34.068589551019997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A6" s="61" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="62" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>34.460071724369399</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A7" s="61" t="s">
         <v>38</v>
       </c>
       <c r="B7" s="62" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C7">
+        <v>33.438862066676201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="63" t="s">
         <v>40</v>
       </c>
       <c r="B8" s="64" t="s">
         <v>41</v>
+      </c>
+      <c r="C8">
+        <v>32.722643513289803</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="20.25" x14ac:dyDescent="0.3">
@@ -4021,7 +4044,7 @@
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView topLeftCell="A33" zoomScale="85" workbookViewId="0">
-      <selection activeCell="L53" sqref="L53"/>
+      <selection activeCell="L55" sqref="L55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4594,7 +4617,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="51">
-        <v>5.8995899999999999</v>
+        <v>3.04867</v>
       </c>
       <c r="C40" s="49">
         <f>B33</f>
@@ -4614,7 +4637,7 @@
         <v>27</v>
       </c>
       <c r="B41" s="51">
-        <v>0.22700500000000001</v>
+        <v>0.16231799999999999</v>
       </c>
       <c r="C41" s="49">
         <v>0</v>
@@ -4631,7 +4654,7 @@
         <v>28</v>
       </c>
       <c r="B42" s="51">
-        <v>-5.3392200000000001</v>
+        <v>-2.7215099999999999</v>
       </c>
       <c r="C42" s="49">
         <f>B35</f>
@@ -4652,7 +4675,7 @@
       </c>
       <c r="M45" s="14">
         <f>SLOPE(C40:C42,B40:B42)</f>
-        <v>16.917487903346107</v>
+        <v>32.951978266894642</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
@@ -4661,7 +4684,7 @@
       </c>
       <c r="M46" s="14">
         <f>RSQ(C40:C42,B40:B42)</f>
-        <v>0.99996130668114824</v>
+        <v>0.99999898151009714</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
@@ -4670,7 +4693,7 @@
       </c>
       <c r="M47" s="14">
         <f>330/M45</f>
-        <v>19.506442202611499</v>
+        <v>10.01457324738333</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
@@ -4679,7 +4702,7 @@
       </c>
       <c r="M48" s="14">
         <f>-(-10-B41)*M45</f>
-        <v>173.01523337496016</v>
+        <v>334.86848187727225</v>
       </c>
     </row>
     <row r="49" spans="12:13" x14ac:dyDescent="0.2">
@@ -4688,7 +4711,7 @@
       </c>
       <c r="M49" s="14">
         <f>-(10-B41)*M45</f>
-        <v>-165.33452469196197</v>
+        <v>-324.17108346062059</v>
       </c>
     </row>
     <row r="51" spans="12:13" x14ac:dyDescent="0.2">
@@ -4713,7 +4736,7 @@
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView topLeftCell="A37" zoomScale="85" workbookViewId="0">
-      <selection activeCell="L53" sqref="L53"/>
+      <selection activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5286,7 +5309,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="51">
-        <v>5.9729999999999999</v>
+        <v>2.9597000000000002</v>
       </c>
       <c r="C40" s="49">
         <f>B33</f>
@@ -5306,7 +5329,7 @@
         <v>27</v>
       </c>
       <c r="B41" s="51">
-        <v>0.16631899999999999</v>
+        <v>7.0880299999999993E-2</v>
       </c>
       <c r="C41" s="49">
         <v>0</v>
@@ -5323,7 +5346,7 @@
         <v>28</v>
       </c>
       <c r="B42" s="51">
-        <v>-5.6299400000000004</v>
+        <v>-2.8110200000000001</v>
       </c>
       <c r="C42" s="49">
         <f>B35</f>
@@ -5344,7 +5367,7 @@
       </c>
       <c r="M45" s="14">
         <f>SLOPE(C40:C42,B40:B42)</f>
-        <v>16.47982102341377</v>
+        <v>33.135271036646103</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
@@ -5353,7 +5376,7 @@
       </c>
       <c r="M46" s="14">
         <f>RSQ(C40:C42,B40:B42)</f>
-        <v>0.99999964734397695</v>
+        <v>0.99999982346319549</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
@@ -5362,7 +5385,7 @@
       </c>
       <c r="M47" s="14">
         <f>330/M45</f>
-        <v>20.024489315214723</v>
+        <v>9.9591761188563996</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
@@ -5371,7 +5394,7 @@
       </c>
       <c r="M48" s="14">
         <f>-(-10-B41)*M45</f>
-        <v>167.53911758693084</v>
+        <v>333.70134831811981</v>
       </c>
     </row>
     <row r="49" spans="12:13" x14ac:dyDescent="0.2">
@@ -5380,7 +5403,7 @@
       </c>
       <c r="M49" s="14">
         <f>-(10-B41)*M45</f>
-        <v>-162.05730288134455</v>
+        <v>-329.00407241480224</v>
       </c>
     </row>
     <row r="51" spans="12:13" x14ac:dyDescent="0.2">
@@ -5404,8 +5427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="85" workbookViewId="0">
-      <selection activeCell="M51" sqref="M51"/>
+    <sheetView topLeftCell="A34" zoomScale="85" workbookViewId="0">
+      <selection activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5978,7 +6001,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="51">
-        <v>6.0389999999999997</v>
+        <v>2.99234</v>
       </c>
       <c r="C40" s="49">
         <f>B33</f>
@@ -5998,7 +6021,7 @@
         <v>27</v>
       </c>
       <c r="B41" s="51">
-        <v>0.26349699999999998</v>
+        <v>0.175562</v>
       </c>
       <c r="C41" s="49">
         <v>0</v>
@@ -6015,7 +6038,7 @@
         <v>28</v>
       </c>
       <c r="B42" s="51">
-        <v>-5.5067399999999997</v>
+        <v>-2.6374499999999999</v>
       </c>
       <c r="C42" s="49">
         <f>B35</f>
@@ -6036,7 +6059,7 @@
       </c>
       <c r="M45" s="14">
         <f>SLOPE(C40:C42,B40:B42)</f>
-        <v>16.612097781298012</v>
+        <v>34.068589551019969</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
@@ -6045,7 +6068,7 @@
       </c>
       <c r="M46" s="14">
         <f>RSQ(C40:C42,B40:B42)</f>
-        <v>0.99999512606497887</v>
+        <v>0.999995653547882</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
@@ -6054,7 +6077,7 @@
       </c>
       <c r="M47" s="14">
         <f>330/M45</f>
-        <v>19.865040788016294</v>
+        <v>9.6863417109124264</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
@@ -6063,7 +6086,7 @@
       </c>
       <c r="M48" s="14">
         <f>-(-10-B41)*M45</f>
-        <v>170.49821574205879</v>
+        <v>346.66704522895583</v>
       </c>
     </row>
     <row r="49" spans="12:13" x14ac:dyDescent="0.2">
@@ -6072,7 +6095,7 @@
       </c>
       <c r="M49" s="14">
         <f>-(10-B41)*M45</f>
-        <v>-161.74373988390144</v>
+        <v>-334.70474579144354</v>
       </c>
     </row>
     <row r="51" spans="12:13" x14ac:dyDescent="0.2">
@@ -6097,7 +6120,7 @@
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView topLeftCell="A31" zoomScale="85" workbookViewId="0">
-      <selection activeCell="M51" sqref="M51"/>
+      <selection activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6670,7 +6693,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="51">
-        <v>6.3773400000000002</v>
+        <v>3.2391299999999998</v>
       </c>
       <c r="C40" s="49">
         <f>B33</f>
@@ -6690,7 +6713,7 @@
         <v>27</v>
       </c>
       <c r="B41" s="51">
-        <v>0.64461900000000005</v>
+        <v>0.440218</v>
       </c>
       <c r="C41" s="49">
         <v>0</v>
@@ -6707,7 +6730,7 @@
         <v>28</v>
       </c>
       <c r="B42" s="51">
-        <v>-5.09063</v>
+        <v>-2.3597700000000001</v>
       </c>
       <c r="C42" s="49">
         <f>B35</f>
@@ -6728,7 +6751,7 @@
       </c>
       <c r="M45" s="14">
         <f>SLOPE(C40:C42,B40:B42)</f>
-        <v>16.824118713985666</v>
+        <v>34.460071724369449</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
@@ -6737,7 +6760,7 @@
       </c>
       <c r="M46" s="14">
         <f>RSQ(C40:C42,B40:B42)</f>
-        <v>0.99999568389398874</v>
+        <v>0.99999575141975972</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
@@ -6746,7 +6769,7 @@
       </c>
       <c r="M47" s="14">
         <f>330/M45</f>
-        <v>19.614697542860025</v>
+        <v>9.5763004395208746</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
@@ -6755,7 +6778,7 @@
       </c>
       <c r="M48" s="14">
         <f>-(-10-B41)*M45</f>
-        <v>179.08633372114738</v>
+        <v>359.77066109805293</v>
       </c>
     </row>
     <row r="49" spans="12:13" x14ac:dyDescent="0.2">
@@ -6764,7 +6787,7 @@
       </c>
       <c r="M49" s="14">
         <f>-(10-B41)*M45</f>
-        <v>-157.39604055856591</v>
+        <v>-329.43077338933603</v>
       </c>
     </row>
     <row r="51" spans="12:13" x14ac:dyDescent="0.2">
@@ -6788,8 +6811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="85" workbookViewId="0">
-      <selection activeCell="M51" sqref="M51"/>
+    <sheetView topLeftCell="A27" zoomScale="85" workbookViewId="0">
+      <selection activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7362,7 +7385,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="51">
-        <v>6.3040200000000004</v>
+        <v>3.1473599999999999</v>
       </c>
       <c r="C40" s="49">
         <f>B33</f>
@@ -7382,7 +7405,7 @@
         <v>27</v>
       </c>
       <c r="B41" s="51">
-        <v>0.53485099999999997</v>
+        <v>0.282163</v>
       </c>
       <c r="C41" s="49">
         <v>0</v>
@@ -7399,7 +7422,7 @@
         <v>28</v>
       </c>
       <c r="B42" s="51">
-        <v>-5.2269399999999999</v>
+        <v>-2.5787399999999998</v>
       </c>
       <c r="C42" s="49">
         <f>B35</f>
@@ -7420,7 +7443,7 @@
       </c>
       <c r="M45" s="14">
         <f>SLOPE(C40:C42,B40:B42)</f>
-        <v>16.605233842836896</v>
+        <v>33.438862066676194</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
@@ -7429,7 +7452,7 @@
       </c>
       <c r="M46" s="14">
         <f>RSQ(C40:C42,B40:B42)</f>
-        <v>0.99999869759212623</v>
+        <v>0.99999854852393466</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
@@ -7438,7 +7461,7 @@
       </c>
       <c r="M47" s="14">
         <f>330/M45</f>
-        <v>19.873252200079929</v>
+        <v>9.8687568776111121</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
@@ -7447,7 +7470,7 @@
       </c>
       <c r="M48" s="14">
         <f>-(-10-B41)*M45</f>
-        <v>174.93366435444412</v>
+        <v>343.82383030408153</v>
       </c>
     </row>
     <row r="49" spans="12:13" x14ac:dyDescent="0.2">
@@ -7456,7 +7479,7 @@
       </c>
       <c r="M49" s="14">
         <f>-(10-B41)*M45</f>
-        <v>-157.17101250229379</v>
+        <v>-324.95341102944235</v>
       </c>
     </row>
     <row r="51" spans="12:13" x14ac:dyDescent="0.2">
@@ -7480,8 +7503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" workbookViewId="0">
-      <selection activeCell="M47" sqref="M47"/>
+    <sheetView topLeftCell="A33" zoomScale="85" workbookViewId="0">
+      <selection activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8054,7 +8077,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="51">
-        <v>6.2019099999999998</v>
+        <v>3.1657099999999998</v>
       </c>
       <c r="C40" s="49">
         <f>B33</f>
@@ -8074,7 +8097,7 @@
         <v>27</v>
       </c>
       <c r="B41" s="51">
-        <v>0.466248</v>
+        <v>0.261407</v>
       </c>
       <c r="C41" s="49">
         <v>0</v>
@@ -8091,7 +8114,7 @@
         <v>28</v>
       </c>
       <c r="B42" s="51">
-        <v>-5.2678000000000003</v>
+        <v>-2.6425100000000001</v>
       </c>
       <c r="C42" s="49">
         <f>B35</f>
@@ -8112,7 +8135,7 @@
       </c>
       <c r="M45" s="14">
         <f>SLOPE(C40:C42,B40:B42)</f>
-        <v>16.570631156612254</v>
+        <v>32.722643513289796</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
@@ -8121,7 +8144,7 @@
       </c>
       <c r="M46" s="14">
         <f>RSQ(C40:C42,B40:B42)</f>
-        <v>0.99999291561955894</v>
+        <v>0.99999268554798726</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
@@ -8130,7 +8153,7 @@
       </c>
       <c r="M47" s="14">
         <f>330/M45</f>
-        <v>19.914751398489646</v>
+        <v>10.084759804505881</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
@@ -8139,7 +8162,7 @@
       </c>
       <c r="M48" s="14">
         <f>-(-10-B41)*M45</f>
-        <v>173.43233520163071</v>
+        <v>335.7803632057765</v>
       </c>
     </row>
     <row r="49" spans="12:13" x14ac:dyDescent="0.2">
@@ -8148,7 +8171,7 @@
       </c>
       <c r="M49" s="14">
         <f>-(10-B41)*M45</f>
-        <v>-157.9802879306144</v>
+        <v>-318.67250706001943</v>
       </c>
     </row>
     <row r="51" spans="12:13" x14ac:dyDescent="0.2">

</xml_diff>